<commit_message>
MenuDocente (modificar docente e inscribir a curso)
falta todo el tema de la gestion de las notas
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>ESTADO</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Averiguar: ¿Los reportes son para los ADMIN o para los PROFESORES?</t>
+  </si>
+  <si>
+    <t>En "DocenteCursoABM" el combo box curso debe mejorarse!</t>
+  </si>
+  <si>
+    <t>En "MenuDocente" el combo box de los cursos debe mejorarse!</t>
+  </si>
+  <si>
+    <t>En "MenuDocente" el boton de "gestionar notas" debe redirigir  al form "CargarNotasCurso".</t>
   </si>
 </sst>
 </file>
@@ -481,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -601,7 +610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="30">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
         <v>18</v>
@@ -629,15 +638,23 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2"/>

</xml_diff>

<commit_message>
En usuariosABM se autocompletan algunos campos
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>ESTADO</t>
   </si>
@@ -84,9 +84,6 @@
     <t>IMPORTANTE</t>
   </si>
   <si>
-    <t>Averiguar: Cómo deberia ser el uso del sistema para los profesores.</t>
-  </si>
-  <si>
     <t>Averiguar: ¿Los reportes son para los ADMIN o para los PROFESORES?</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>En "MenuDocente" el boton de "gestionar notas" debe redirigir  al form "CargarNotasCurso".</t>
+  </si>
+  <si>
+    <t>Averiguar: Cómo deberia ser el uso del sistema para los profesores. A partir de aca seguir con la carga de NOTAS!</t>
   </si>
 </sst>
 </file>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -599,7 +599,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
@@ -625,27 +625,29 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B21" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -653,7 +655,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2">

</xml_diff>

<commit_message>
Extended todas las clases que lo necesitaban
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -72,9 +72,6 @@
     <t>Un alumno y un profesor que tengan cuentas de usuario deberian poder modificar su clave y otros datos de usuario si lo desean.</t>
   </si>
   <si>
-    <t>Averiguar: ¿Qué es "año especialidad" en el alta de comisiones?</t>
-  </si>
-  <si>
     <t>IMPORTANTE</t>
   </si>
   <si>
@@ -94,13 +91,16 @@
   </si>
   <si>
     <t>En la "InscripcionAlumnoABM" (inscripcion a un curso) se debe validar que haya cupo!!</t>
+  </si>
+  <si>
+    <t>Averiguar: ¿Qué es "año especialidad" en el alta de comisiones? El año de la carrera (1ro, 2do, …, 5to)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +112,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +193,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -518,117 +526,119 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30">
+      <c r="A18" s="2"/>
       <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
@@ -640,18 +650,16 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2"/>
@@ -864,10 +872,6 @@
     <row r="78" spans="1:2">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bugs varios OK (relacionados a las clases extended)
En el proximo commit veo si arreglo el temita de los profes al
inscribirse a cursos
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>ESTADO</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Averiguar: ¿Qué es "año especialidad" en el alta de comisiones? El año de la carrera (1ro, 2do, …, 5to)</t>
+  </si>
+  <si>
+    <t>Deshabilitar legajo en personaABM modificar</t>
+  </si>
+  <si>
+    <t>UsuarioABM alta mejorar combobox</t>
+  </si>
+  <si>
+    <t>Listar planes, materias, comisiones, cursos,  edit y elim crash</t>
   </si>
 </sst>
 </file>
@@ -495,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -586,7 +595,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
@@ -624,7 +633,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -650,7 +659,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -658,16 +667,22 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2"/>

</xml_diff>

<commit_message>
Bug de la inscripcion de profes a curso OK
Checkealo marce por las dudas, pero aca parece que se solucionó.
Hay validaciones para hacer, y despues los reportes y ya casi estariamos
con el desktop.
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>ESTADO</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Listar planes, materias, comisiones, cursos,  edit y elim crash</t>
+  </si>
+  <si>
+    <t>validar DocenteCursoABM (validar campos y que el docente no se inscriba 2 veces en un mismo curso)</t>
+  </si>
+  <si>
+    <t>Armar al menos 2 reportes (se me ocurre "alumnos con mejor promedio de estado academico" y "profesores con mayor carga horaria")</t>
   </si>
 </sst>
 </file>
@@ -504,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -686,11 +692,15 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30">
       <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2"/>

</xml_diff>

<commit_message>
menues web en progreso
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -691,7 +691,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Emm me comi commitear esto
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>ESTADO</t>
   </si>
@@ -109,6 +109,30 @@
   </si>
   <si>
     <t>Armar al menos 2 reportes (se me ocurre "alumnos con mejor promedio de estado academico" y "profesores con mayor carga horaria")</t>
+  </si>
+  <si>
+    <t>WEB: Login</t>
+  </si>
+  <si>
+    <t>WEB: Modificar datos (ya sea admin, profe o alumno)</t>
+  </si>
+  <si>
+    <t>WEB: Estado academico (alumno)</t>
+  </si>
+  <si>
+    <t>WEB: Inscripcion a materia (alumno)</t>
+  </si>
+  <si>
+    <t>WEB: falta validar "ModificarDatos.aspx"</t>
+  </si>
+  <si>
+    <t>WEB: Cargar notas (profe)</t>
+  </si>
+  <si>
+    <t>WEB: Inscribirse a curso (profe)</t>
+  </si>
+  <si>
+    <t>WEB: ABMs del admin (son un monton!!)</t>
   </si>
 </sst>
 </file>
@@ -510,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -703,36 +727,52 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
+      <c r="B37" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2"/>

</xml_diff>

<commit_message>
TODO update (no agregue nada)
</commit_message>
<xml_diff>
--- a/TODO LIST.xlsx
+++ b/TODO LIST.xlsx
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -799,13 +799,13 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="2"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="2"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="3" t="s">
         <v>40</v>
       </c>
@@ -817,13 +817,13 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="2"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="2"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="3" t="s">
         <v>42</v>
       </c>

</xml_diff>